<commit_message>
added the v2 of the app with major modifications
</commit_message>
<xml_diff>
--- a/data/HW_list.xlsx
+++ b/data/HW_list.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C123"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="C119" sqref="C117:C119"/>
@@ -463,7 +463,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>King Kuda</t>
+          <t>Ford Mustang Dark Horse</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -478,7 +478,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ford Mustang Dark Horse</t>
+          <t>McLaren F1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -493,7 +493,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>McLaren F1</t>
+          <t>96 Porsche Carrera</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -508,7 +508,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>96 Porsche Carrera</t>
+          <t>Shelby Cobra "Daytona" Coupe</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Shelby Cobra "Daytona" Coupe</t>
+          <t>98 Subaru Impreza 22B Sti Version</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>98 Subaru Impreza 22B Sti Version</t>
+          <t>Tesla CyberTruck</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Tesla CyberTruck</t>
+          <t xml:space="preserve">Bugatti Bolide </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bugatti Bolide </t>
+          <t>Alfa Romeo GTV6 3.0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Alfa Romeo GTV6 3.0</t>
+          <t>91 Mazda MX-5 Miata</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -598,7 +598,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>91 Mazda MX-5 Miata</t>
+          <t>90 Acura NSX</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>90 Acura NSX</t>
+          <t>Nissan Skyline GT-R (BNR32)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Nissan Skyline GT-R (BNR32)</t>
+          <t>Tesla Model S Plaid</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Tesla Model S Plaid</t>
+          <t>Lamborghini Huracan LP 620-2 Super Trofeo</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -658,7 +658,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Lamborghini Huracan LP 620-2 Super Trofeo</t>
+          <t>Gordon Murray Automotive T.50s</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Gordon Murray Automotive T.50s</t>
+          <t>LB-Silhouette Works GT Nissan 35GT-RR Ver.2</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>LB-Silhouette Works GT Nissan 35GT-RR Ver.2</t>
+          <t>Lamborghini Sesto Elemento</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Lamborghini Sesto Elemento</t>
+          <t>Lamborghini Huracan Sterrato</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -718,7 +718,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Lamborghini Huracan Sterrato</t>
+          <t>17 Acura NSX</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -733,7 +733,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>17 Acura NSX</t>
+          <t>Corvette C8.R</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -748,7 +748,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Corvette C8.R</t>
+          <t>Aston Martin Vantage GTE</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Aston Martin Vantage GTE</t>
+          <t xml:space="preserve">McLaren Senna </t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -778,7 +778,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">McLaren Senna </t>
+          <t>20 Jaguar F-Type</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -793,7 +793,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>20 Jaguar F-Type</t>
+          <t>Cadillac Project GTP Hypercar</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -808,12 +808,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Muscle And Blown</t>
+          <t>17 Audi RS 6 Avant</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Premiums Pop Culture</t>
         </is>
       </c>
     </row>
@@ -823,12 +823,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Ravenger S/T</t>
+          <t>BMW M4</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Silver Series BMW</t>
         </is>
       </c>
     </row>
@@ -838,12 +838,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Cadillac Project GTP Hypercar</t>
+          <t>2016 BMW M2</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Silver Series BMW</t>
         </is>
       </c>
     </row>
@@ -853,12 +853,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>17 Audi RS 6 Avant</t>
+          <t>BMW M1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Premiums Pop Culture</t>
+          <t>Silver Series BMW</t>
         </is>
       </c>
     </row>
@@ -868,12 +868,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BMW M4</t>
+          <t>Batman: Arkham Knight Batmobile</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Silver Series BMW</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -883,12 +883,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2016 BMW M2</t>
+          <t>Batman &amp; Robin Batmobile</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Silver Series BMW</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -898,12 +898,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>BMW M1</t>
+          <t>The Dark Knight Batmobile</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Silver Series BMW</t>
+          <t>Premiums Pop Culture</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Batman: Arkham Knight Batmobile</t>
+          <t>08 Dodge Challenger SRT8</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -928,7 +928,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Batman &amp; Robin Batmobile</t>
+          <t xml:space="preserve">70 Dodge Hemi Challenger </t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -943,12 +943,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>The Dark Knight Batmobile</t>
+          <t>Dodge Viper GTS-R</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Premiums Pop Culture</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -958,7 +958,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>08 Dodge Challenger SRT8</t>
+          <t>78 Dodge Li'l Red Express Truck</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -973,7 +973,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve">70 Dodge Hemi Challenger </t>
+          <t>69 Dodge Charger Daytona</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -988,7 +988,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Dodge Viper GTS-R</t>
+          <t>21 Ford Bronco</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1003,12 +1003,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>78 Dodge Li'l Red Express Truck</t>
+          <t>Porsche 934 Turbo RSR</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Neon Speeders</t>
         </is>
       </c>
     </row>
@@ -1018,12 +1018,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>69 Dodge Charger Daytona</t>
+          <t>Datsun Fairlady 2000</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Neon Speeders</t>
         </is>
       </c>
     </row>
@@ -1033,12 +1033,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Mod Speeder</t>
+          <t>Mazda RX-7</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Neon Speeders</t>
         </is>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>21 Ford Bronco</t>
+          <t>Aston Martin DB4GT High-Speed Edition</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1063,12 +1063,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Porsche 934 Turbo RSR</t>
+          <t>Ford Mustang Mach-E 1400</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Neon Speeders</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -1078,12 +1078,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Datsun Fairlady 2000</t>
+          <t>Mustang Mach 1</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Neon Speeders</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -1093,12 +1093,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Mazda RX-7</t>
+          <t>Lamborghini Countach Pace Car</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Neon Speeders</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Aston Martin DB4GT High-Speed Edition</t>
+          <t>Porsche 917LH</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Ford Mustang Mach-E 1400</t>
+          <t>Volkswagen Beetle (Bumblebee)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1138,12 +1138,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Mustang Mach 1</t>
+          <t>70 Ford Escort RS1600</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Ultra Hots</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Lamborghini Countach Pace Car</t>
+          <t>Humvee</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Porsche 917LH</t>
+          <t>McLaren P1</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Erikenstein Rod</t>
+          <t>Lotus Emira</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Head Starter</t>
+          <t>K.I.T.T.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Volkswagen Beetle (Bumblebee)</t>
+          <t>95 Mazda RX-7</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Purple Passion</t>
+          <t>Toyota GR86 Cup</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1243,12 +1243,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>70 Ford Escort RS1600</t>
+          <t>BMW i8 Roadster</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Ultra Hots</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -1258,7 +1258,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Humvee</t>
+          <t>Lamborghini Gallardo LP 570-4 Superleggera</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>McLaren P1</t>
+          <t>20 Toyota GR Supra</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Lotus Emira</t>
+          <t>Dimachinni Veloce</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>K.I.T.T.</t>
+          <t>87 Ford Sierra Cosworth</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>95 Mazda RX-7</t>
+          <t>Nissan Maxima Drift Car</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Toyota GR86 Cup</t>
+          <t>Subaru WRX STI</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1348,12 +1348,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>BMW i8 Roadster</t>
+          <t>Porsche Cayman S</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>57th Anniversary Series</t>
         </is>
       </c>
     </row>
@@ -1363,12 +1363,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Mod Speeder</t>
+          <t>Shelby Cobra 427 S/C</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>57th Anniversary Series</t>
         </is>
       </c>
     </row>
@@ -1378,12 +1378,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Lamborghini Gallardo LP 570-4 Superleggera</t>
+          <t>Custom '68 Camaro</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>57th Anniversary Series</t>
         </is>
       </c>
     </row>
@@ -1393,12 +1393,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>20 Toyota GR Supra</t>
+          <t>Porsche 356 Outlaw</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Ultra Hots</t>
         </is>
       </c>
     </row>
@@ -1408,12 +1408,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Dimachinni Veloce</t>
+          <t>05 Aston Martin DB9</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Silver Series Fast &amp; Furious Villains</t>
         </is>
       </c>
     </row>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>87 Ford Sierra Cosworth</t>
+          <t>87 Audi Quattro</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Nissan Maxima Drift Car</t>
+          <t>Dodge Viper RT/10</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Subaru WRX STI</t>
+          <t xml:space="preserve">Ford GT LM </t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1468,12 +1468,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Porsche Cayman S</t>
+          <t>67 Ford GT40 Mk.IV</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>57th Anniversary Series</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -1483,12 +1483,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Shelby Cobra 427 S/C</t>
+          <t>Porsche 904 Carrera GTS</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>57th Anniversary Series</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -1498,12 +1498,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Custom '68 Camaro</t>
+          <t>Porsche 911 Turbo (930)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>57th Anniversary Series</t>
+          <t>Premiums Pop Culture</t>
         </is>
       </c>
     </row>
@@ -1513,12 +1513,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Porsche 356 Outlaw</t>
+          <t>Delorean Alpha5</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Ultra Hots</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -1528,12 +1528,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>05 Aston Martin DB9</t>
+          <t>15 Jaguar F-Type Project 7</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Silver Series Fast &amp; Furious Villains</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -1543,12 +1543,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>87 Audi Quattro</t>
+          <t>Volkswagen "Baja Bug"</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>57th Anniversary Series</t>
         </is>
       </c>
     </row>
@@ -1558,12 +1558,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Dodge Viper RT/10</t>
+          <t>55 Corvette</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>57th Anniversary Series</t>
         </is>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Hako Type D</t>
+          <t>Czinger 21C</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ford GT LM </t>
+          <t>16 Ford GT Race</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>67 Ford GT40 Mk.IV</t>
+          <t>17 Ford GT</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1618,7 +1618,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Porsche 904 Carrera GTS</t>
+          <t>Automobili Pininfarina Battista</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -1633,12 +1633,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Porsche 911 Turbo (930)</t>
+          <t>Rimac Revera</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Premiums Pop Culture</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Delorean Alpha5</t>
+          <t>McLaren Speedtail</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>15 Jaguar F-Type Project 7</t>
+          <t>Pagani Zonda R</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -1678,12 +1678,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Volkswagen "Baja Bug"</t>
+          <t>Aston Martin V8 Vantage</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>57th Anniversary Series</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -1693,12 +1693,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>55 Corvette</t>
+          <t>20 Ford Mustang Shelby GT500</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>57th Anniversary Series</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -1708,7 +1708,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Amaru GTC</t>
+          <t>Porsche 911 GT3</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -1723,12 +1723,12 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Decidedly Go</t>
+          <t>Porsche 918 Spyder</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>1/4 Mile Finals Series</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Czinger 21C</t>
+          <t>McLaren W1</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Rrroadster</t>
+          <t>95 Mazda RX-7 Drift</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -1766,9 +1766,9 @@
       <c r="A90" t="n">
         <v>89</v>
       </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>16 Ford GT Race</t>
+      <c r="B90" s="1" t="inlineStr">
+        <is>
+          <t>71 Lamborghini Miura SV</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -1783,12 +1783,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>17 Ford GT</t>
+          <t>Mazda RX-3</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>HW Speed Graphics</t>
         </is>
       </c>
     </row>
@@ -1798,7 +1798,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Automobili Pininfarina Battista</t>
+          <t>Maserati Shamal</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Rimac Revera</t>
+          <t>CUPRA e-Racer</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -1826,9 +1826,9 @@
       <c r="A94" t="n">
         <v>93</v>
       </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>McLaren Speedtail</t>
+      <c r="B94" s="1" t="inlineStr">
+        <is>
+          <t>15 Ford Mustang GT Convertible</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Pagani Zonda R</t>
+          <t>Aston Martin One-77</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -1858,7 +1858,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Aston Martin V8 Vantage</t>
+          <t>McLaren Solus GT</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -1873,7 +1873,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>20 Ford Mustang Shelby GT500</t>
+          <t>Mazda 787B</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Porsche 911 GT3</t>
+          <t>Nissan Leaf Nismo RC_02</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -1903,12 +1903,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Porsche 918 Spyder</t>
+          <t>De Tomaso Pantera Gruppo 4</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>1/4 Mile Finals Series</t>
+          <t>Premiums Boulevard</t>
         </is>
       </c>
     </row>
@@ -1918,12 +1918,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>McLaren W1</t>
+          <t>Porsche 718 Cayman GT4</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Premiums Boulevard</t>
         </is>
       </c>
     </row>
@@ -1933,12 +1933,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>95 Mazda RX-7 Drift</t>
+          <t>Lamborghini Countach LPI 800-4</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Premiums Boulevard</t>
         </is>
       </c>
     </row>
@@ -1946,9 +1946,9 @@
       <c r="A102" t="n">
         <v>101</v>
       </c>
-      <c r="B102" s="1" t="inlineStr">
-        <is>
-          <t>71 Lamborghini Miura SV</t>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Ferrari SF90 Stradale</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -1963,12 +1963,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Mazda RX-3</t>
+          <t>67 Mustang</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>HW Speed Graphics</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -1978,7 +1978,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Maserati Shamal</t>
+          <t>71 Mustang Funny Car</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>CUPRA e-Racer</t>
+          <t>Audi 90 Quattro</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2006,9 +2006,9 @@
       <c r="A106" t="n">
         <v>105</v>
       </c>
-      <c r="B106" s="1" t="inlineStr">
-        <is>
-          <t>15 Ford Mustang GT Convertible</t>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>89 Mercedes-Benz 560 SEC AMG</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2023,12 +2023,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Aston Martin One-77</t>
+          <t>Mclaren 720S</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Fast &amp; Furious Hobbs &amp; Shaw</t>
         </is>
       </c>
     </row>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>McLaren Solus GT</t>
+          <t>Ferrari 365 GTB4 Competizione</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Mazda 787B</t>
+          <t>Porsche 911 GT3 RS</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Nissan Leaf Nismo RC_02</t>
+          <t>Pagani Utopia</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2083,12 +2083,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>De Tomaso Pantera Gruppo 4</t>
+          <t>17 Pagani Huayra Roadster</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Premiums Boulevard</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -2098,12 +2098,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Porsche 718 Cayman GT4</t>
+          <t>Ferrari F40 Competizione</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Premiums Boulevard</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -2113,12 +2113,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Lamborghini Countach LPI 800-4</t>
+          <t>BMW 2002</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Premiums Boulevard</t>
+          <t>Neon Speeders</t>
         </is>
       </c>
     </row>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Ferrari SF90 Stradale</t>
+          <t>Porsche 911 Carrera RS 2.7</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2143,12 +2143,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>67 Mustang</t>
+          <t>Porsche 911 Carrera RS 3.8</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Premiums Fast &amp; Furious</t>
         </is>
       </c>
     </row>
@@ -2158,12 +2158,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>71 Mustang Funny Car</t>
+          <t>95 Lamborghini Diablo SV</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Premiums Boulevard</t>
         </is>
       </c>
     </row>
@@ -2173,12 +2173,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Audi 90 Quattro</t>
+          <t>BMW 320 Group 5</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Premiums Car Culture</t>
         </is>
       </c>
     </row>
@@ -2188,12 +2188,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>89 Mercedes-Benz 560 SEC AMG</t>
+          <t>2001 BMW M3 GTR</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Mainlines</t>
+          <t>Premiums Car Culture</t>
         </is>
       </c>
     </row>
@@ -2203,12 +2203,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Mclaren 720S</t>
+          <t>BMW M3 GT2</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Fast &amp; Furious Hobbs &amp; Shaw</t>
+          <t>Mainlines</t>
         </is>
       </c>
     </row>
@@ -2218,7 +2218,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Ferrari 365 GTB4</t>
+          <t>73 BMW 3.0 CSL Race Car</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Porsche 911 GT3 RS</t>
+          <t>BMW 635 CSi</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Pagani Utopia</t>
+          <t>16 Mercedes-AMG GT3</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -2263,10 +2263,895 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>17 Pagani Huayra Roadster</t>
+          <t>Mercedes-Benz 500 E</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>123</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Lamborghini Veneno</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>124</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>McLaren Elva</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>125</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Lamborghini Sian FKP 37</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>126</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Alfa Romeo 8C Competizione</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>127</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Jaguar MK1</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>128</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Jaguar XJC V12 Coupe</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>129</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Datsun 240Z</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>130</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>94 Bugatti EB110 SS</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>131</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>16 Bugatti Chiron</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>132</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Porsche 935</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>133</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Porsche 993 GT2</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>134</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>2019 Audi R8 Spyder</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>135</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>84 Mustang SVO</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>136</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>92 Ford Mustang</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>137</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Custom '18 Ford Mustang GT</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>138</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>10 Ford Shelby GT-500 Super Snake</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>139</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Lamborghini Reventon Roadster</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>140</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Lamborghini Aventador J</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>141</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Koenigsegg Gemera</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>142</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Alfa Romeo Guilia Ti Super</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>143</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>65 Ford Mustang Convertible</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>144</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>84 Audi Sport Quattro</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Aston Martin V12 Speedster</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Premiums Car Culture</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>146</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>67 Porsche 911 R</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Silver Series National Icons</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>147</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Porsche Panamera Turbo S E-Hybrid Sport Turismo</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Luxury Sedans</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Toyota Supra</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Premiums Car Culture</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Toyota 2000GT</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Premiums Car Culture</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Cadillac CTS-V</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Luxury Sedans</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>16 Cadillac ATS-V R</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Porsche Panamera</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>82 Toyota Supra</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>154</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Nissan Skyline RS (KDR30)</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>155</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Nissan Skyline 2000 GT-R</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>54th Anniversary Series</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>156</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>1970 Chevrolet Chevelle SS</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>157</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Corvette C6</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>158</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>72 Stingray Convertible</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>159</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>DMC DeLorean</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>160</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>69 Camaro</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>161</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>2018 Ford Mustang GT</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>162</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Custom '15 Ford Mustang</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>163</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Porsche Safari</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Track Fleet</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>164</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Audi RS 5 Coupe</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>165</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Porsche Boxster Spyder</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>166</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>19 Chevrolet Corvette ZR1 Convertible</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>167</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Corvette C7 Z06</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>168</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>89 Mazda Savanna RX-7 FC3S</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>169</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Lamborghini Essenza SCV12</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Premiums Car Culture</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>170</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Subaru BRZ Pandem</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>171</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Custom Kia EV6</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>172</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Ford Escort</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>173</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Ford Model A Custom '31</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>174</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Lotus Cortina</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>175</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Aston Martin Vulcan</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>176</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Lamborghini Huracan LP 610-4</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>177</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Lotus Evija</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>178</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>11 Dodge Charger R/T</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>179</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Morgan Super 3</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>180</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Peugeot 9x8 Hypercar</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>181</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Jaguar XE SV Project 8</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
         <is>
           <t>Mainlines</t>
         </is>

</xml_diff>

<commit_message>
renamed semi premiums to silver series
</commit_message>
<xml_diff>
--- a/data/HW_list.xlsx
+++ b/data/HW_list.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C188"/>
+  <dimension ref="A1:C194"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="C119" sqref="C117:C119"/>
@@ -3247,6 +3247,96 @@
         </is>
       </c>
     </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>188</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Nissan Skyline GT-R (R32)</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Color Shifters</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>189</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Gordon Murray Automotive T.33</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>190</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Porsche 911 Turbo Cabriolet</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>191</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>89 Porsche 944 Turbo</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>192</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>2013 SRT Viper</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>193</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>92 BMW M3</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
shifted the css styling from bootstrap to tailwind and also added pages folder structure
</commit_message>
<xml_diff>
--- a/data/HW_list.xlsx
+++ b/data/HW_list.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C194"/>
+  <dimension ref="A1:C215"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="C119" sqref="C117:C119"/>
@@ -3337,6 +3337,321 @@
         </is>
       </c>
     </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>194</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Batman: Arkham Asylum Batmobile</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>195</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>TV Series Batmobile</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>196</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>The Bat</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>197</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Ford GT-40</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Silver Series National Icons</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>198</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Porsche 914 Safari</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>HW Speed Graphics</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>199</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>16 Lamborghini Centenario Roadster</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>200</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>2018 Bentley Continental GT3</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Premiums Fast &amp; Furious</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>201</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Mazda RX7 FC Pandem</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>Premiums Car Culture</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>202</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>04 Mazda Mazdaspeed Miata</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Premiums Car Culture</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>203</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Audi RS E-Tron GT</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>204</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Maserati MC20</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>Premiums Boulevard</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>205</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>1989 Batmobile</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>206</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Justice League Batmobile</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>207</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Custom Cadillac Fleetwood</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>53rd Anniversary Series</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>208</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Corvette Grand Sport Roadster</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>209</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Porsche 911 Carrera T</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>210</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>37 Bugatti</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>211</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Bentley Continental Supersports</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>Exotics</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>212</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>BMW M3 Wagon</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>213</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Volvo 240 Drift Wagon</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>214</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>2020 Dodge Charger "Hellcat"</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added v2 of the application
</commit_message>
<xml_diff>
--- a/data/HW_list.xlsx
+++ b/data/HW_list.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C225"/>
+  <dimension ref="A1:C280"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="C119" sqref="C117:C119"/>
@@ -448,7 +448,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>20 Koenigsegg Jesko</t>
+          <t>'20 Koenigsegg Jesko</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -493,7 +493,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>96 Porsche Carrera</t>
+          <t>'96 Porsche Carrera</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>98 Subaru Impreza 22B Sti Version</t>
+          <t>'98 Subaru Impreza 22B Sti Version</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>91 Mazda MX-5 Miata</t>
+          <t>'91 Mazda MX-5 Miata</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -598,7 +598,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>90 Acura NSX</t>
+          <t>'90 Acura NSX</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -718,7 +718,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>17 Acura NSX</t>
+          <t>'17 Acura NSX</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -778,7 +778,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>20 Jaguar F-Type</t>
+          <t>'20 Jaguar F-Type</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -808,7 +808,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>17 Audi RS 6 Avant</t>
+          <t>'17 Audi RS 6 Avant</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -838,7 +838,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2016 BMW M2</t>
+          <t>'16 BMW M2</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -913,7 +913,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>08 Dodge Challenger SRT8</t>
+          <t>'08 Dodge Challenger SRT8</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -928,7 +928,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t xml:space="preserve">70 Dodge Hemi Challenger </t>
+          <t xml:space="preserve">'70 Dodge Hemi Challenger </t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -958,7 +958,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>78 Dodge Li'l Red Express Truck</t>
+          <t>'78 Dodge Li'l Red Express Truck</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -973,7 +973,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>69 Dodge Charger Daytona</t>
+          <t>'69 Dodge Charger Daytona</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -988,7 +988,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>21 Ford Bronco</t>
+          <t>'21 Ford Bronco</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>70 Ford Escort RS1600</t>
+          <t>'70 Ford Escort RS1600</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>95 Mazda RX-7</t>
+          <t>'95 Mazda RX-7</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>20 Toyota GR Supra</t>
+          <t>'20 Toyota GR Supra</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>87 Ford Sierra Cosworth</t>
+          <t>'87 Ford Sierra Cosworth</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>05 Aston Martin DB9</t>
+          <t>'05 Aston Martin DB9</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>87 Audi Quattro</t>
+          <t>'87 Audi Quattro</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>67 Ford GT40 Mk.IV</t>
+          <t>'67 Ford GT40 Mk.IV</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>15 Jaguar F-Type Project 7</t>
+          <t>'15 Jaguar F-Type Project 7</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1558,7 +1558,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>55 Corvette</t>
+          <t>'55 Corvette</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>16 Ford GT Race</t>
+          <t>'16 Ford GT Race</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>17 Ford GT</t>
+          <t>'17 Ford GT</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>20 Ford Mustang Shelby GT500</t>
+          <t>'20 Ford Mustang Shelby GT500</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>95 Mazda RX-7 Drift</t>
+          <t>'95 Mazda RX-7 Drift</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="B90" s="1" t="inlineStr">
         <is>
-          <t>71 Lamborghini Miura SV</t>
+          <t>'71 Lamborghini Miura SV</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="B94" s="1" t="inlineStr">
         <is>
-          <t>15 Ford Mustang GT Convertible</t>
+          <t>'15 Ford Mustang GT Convertible</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>67 Mustang</t>
+          <t>'67 Mustang</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -1978,7 +1978,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>71 Mustang Funny Car</t>
+          <t>'71 Mustang Funny Car</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Audi 90 Quattro</t>
+          <t>Audi '90 Quattro</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>89 Mercedes-Benz 560 SEC AMG</t>
+          <t>'89 Mercedes-Benz 560 SEC AMG</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>17 Pagani Huayra Roadster</t>
+          <t>'17 Pagani Huayra Roadster</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2113,7 +2113,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>BMW 2002</t>
+          <t>BMW '02</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2158,7 +2158,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>95 Lamborghini Diablo SV</t>
+          <t>'95 Lamborghini Diablo SV</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>2001 BMW M3 GTR</t>
+          <t>'01 BMW M3 GTR</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -2218,7 +2218,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>73 BMW 3.0 CSL Race Car</t>
+          <t>'73 BMW 3.0 CSL Race Car</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>16 Mercedes-AMG GT3</t>
+          <t>'16 Mercedes-AMG GT3</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -2383,7 +2383,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>94 Bugatti EB110 SS</t>
+          <t>'94 Bugatti EB110 SS</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -2398,7 +2398,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>16 Bugatti Chiron</t>
+          <t>'16 Bugatti Chiron</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Porsche 935 (2022)</t>
+          <t>Porsche 935 ('22)</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -2443,7 +2443,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>2019 Audi R8 Spyder</t>
+          <t>'19 Audi R8 Spyder</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -2458,7 +2458,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>84 Mustang SVO</t>
+          <t>'84 Mustang SVO</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -2473,7 +2473,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>92 Ford Mustang</t>
+          <t>'92 Ford Mustang</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -2503,7 +2503,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>10 Ford Shelby GT-500 Super Snake</t>
+          <t>'10 Ford Shelby GT-500 Super Snake</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -2578,7 +2578,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>65 Ford Mustang Convertible</t>
+          <t>'65 Ford Mustang Convertible</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -2593,7 +2593,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>84 Audi Sport Quattro</t>
+          <t>'84 Audi Sport Quattro</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -2623,7 +2623,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>67 Porsche 911 R</t>
+          <t>'67 Porsche 911 R</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -2698,7 +2698,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>16 Cadillac ATS-V R</t>
+          <t>'16 Cadillac ATS-V R</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>82 Toyota Supra</t>
+          <t>'82 Toyota Supra</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -2758,7 +2758,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Nissan Skyline 2000 GT-R</t>
+          <t>Nissan Skyline 2000GT-R</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -2773,7 +2773,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>1970 Chevrolet Chevelle SS</t>
+          <t>'70 Chevrolet Chevelle SS</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -2803,7 +2803,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>72 Stingray Convertible</t>
+          <t>'72 Stingray Convertible</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>69 Camaro</t>
+          <t>'69 Camaro</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -2848,7 +2848,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>2018 Ford Mustang GT</t>
+          <t>'18 Ford Mustang GT</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Porsche Safari</t>
+          <t>Porsche 911 Off-Roader</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -2923,7 +2923,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>19 Chevrolet Corvette ZR1 Convertible</t>
+          <t>'19 Chevrolet Corvette ZR1 Convertible</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -2953,7 +2953,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>89 Mazda Savanna RX-7 FC3S</t>
+          <t>'89 Mazda Savanna RX-7 FC3S</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -3103,7 +3103,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>11 Dodge Charger R/T</t>
+          <t>'11 Dodge Charger R/T</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Aston Martin 1963 DB5</t>
+          <t>Aston Martin '63 DB5</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -3178,7 +3178,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>71 Porsche 911</t>
+          <t>'71 Porsche 911</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -3208,7 +3208,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>96 Dodge Viper GTS</t>
+          <t>'96 Dodge Viper GTS</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -3298,7 +3298,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>89 Porsche 944 Turbo</t>
+          <t>'89 Porsche 944 Turbo</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>2013 SRT Viper</t>
+          <t>'13 SRT Viper</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -3328,7 +3328,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>92 BMW M3</t>
+          <t>'92 BMW M3</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -3418,7 +3418,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>16 Lamborghini Centenario Roadster</t>
+          <t>'16 Lamborghini Centenario Roadster</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>2018 Bentley Continental GT3</t>
+          <t>'18 Bentley Continental GT3</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -3463,7 +3463,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>04 Mazda Mazdaspeed Miata</t>
+          <t>'04 Mazda Mazdaspeed Miata</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -3508,7 +3508,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>1989 Batmobile</t>
+          <t>'89 Batmobile</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -3583,7 +3583,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>37 Bugatti</t>
+          <t>'37 Bugatti</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -3643,7 +3643,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>2020 Dodge Charger "Hellcat"</t>
+          <t>'20 Dodge Charger "Hellcat"</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -3703,7 +3703,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Porsche 935 (2021)</t>
+          <t>Porsche 935 ('21)</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -3718,7 +3718,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>07 Ford Mustang</t>
+          <t>'07 Ford Mustang</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -3733,7 +3733,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>69 Ford Mustang Boss 302</t>
+          <t>'69 Ford Mustang Boss 302</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -3748,7 +3748,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>2014 Corvette Stingray</t>
+          <t>'14 Corvette Stingray</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -3778,7 +3778,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>49 Drag Merc</t>
+          <t>'49 Drag Merc</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -3797,6 +3797,831 @@
         </is>
       </c>
       <c r="C225" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>225</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Lamborghini Countach LP5000 QV</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>Premiums Car Culture</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>226</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Lancia Stratos Zero</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>Premiums Car Culture</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>227</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Custom '71 El Camino</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>228</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Nissan Skyline GT-R (BCNR33)</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>229</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>'11 Corvette Grand Sport</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>230</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Maserati Quattroporte</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>231</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>'19 Mercedes-Benz A-Class</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>232</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Porsche Carrera GT</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>233</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Jaguar I-Pace eTrophy</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>234</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Dodge Charger Stock Car</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>235</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>BMW 507</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>236</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>'69 Shelby GT-500</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>237</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>Mercedes-Benz 300 SL</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>238</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Porsche 911 GT1 '98</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>239</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Nissan 370Z</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>240</v>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Triumph TR6</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>241</v>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Porsche 911 SC Targa</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>242</v>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Mazda Furai</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>243</v>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>'08 Ford Focus</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>244</v>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Nissan Silvia (S14) Drift</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>56th Anniversary Series</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>245</v>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Porsche 911 GT3 R (992)</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Premiums Car Culture</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>246</v>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>F/A-18E Super Hornet</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>Premiums Pop Culture</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>247</v>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Grumman F-14 Tomcat</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>Premiums Pop Culture</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>248</v>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>'08 Tesla Roadster</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>249</v>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Tesla Model Y</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>250</v>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Tesla Model S</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>251</v>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Corvette C6R</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>252</v>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>'20 Corvette</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>253</v>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>'05 Ford Mustang</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>254</v>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>'81 Camaro</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>255</v>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Tesla Model X</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>256</v>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>BMW 850i</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>257</v>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>'58 Chevy Impala</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>258</v>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>'01 BMW M5 E39</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>Silver Series BMW</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>259</v>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Ferrari 599XX</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>260</v>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Mercedes C-Class</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>261</v>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Porsche 356 Speedster</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>Silver Series Porsche</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>262</v>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>Pontiac Aztek Custom</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>263</v>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Lamborghini Aventador LP 700-4 (Miura Homage)</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>1/4 Mile Finals Series</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>264</v>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>Lamborghini Reventon</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>265</v>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>Lamborghini Estoque</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>266</v>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>'17 Lamborghini Urus</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>267</v>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>'15 Mercedes-AMG GT</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>268</v>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>'67 Ford Mustang Coupe</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>269</v>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Nissan Skyline 2000GT-R LBWK</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>270</v>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>'17 Nissan GT-R (R35)</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>Gran Turismo</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>271</v>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>'96 Nissan 180SX Type X</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>272</v>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Sword Warthog</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>273</v>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Lamborghini LM002</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>Premiums Fast &amp; Furious</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>274</v>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>U.S.S. Enterprise NCC-1701</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>275</v>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Ford Mustang GTD</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>276</v>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>'83 Porsche 928S</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>277</v>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Tesla Model 3</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>278</v>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Ferrari F355 Challenge</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>279</v>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>LB Super Silhouette Nissan Silvia (S15)</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
         <is>
           <t>Mainlines</t>
         </is>

</xml_diff>

<commit_message>
added prorders page t otrack my preorders
</commit_message>
<xml_diff>
--- a/data/HW_list.xlsx
+++ b/data/HW_list.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C280"/>
+  <dimension ref="A1:C289"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="C119" sqref="C117:C119"/>
@@ -4627,6 +4627,141 @@
         </is>
       </c>
     </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>280</v>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>'18 Honda Civic Type R</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>281</v>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Custom Datsun 240Z</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>282</v>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>'71 Nissan Skyline H/T 2000GT-R</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>Silver Series National Icons</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>283</v>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>Nissan Silvia (S15)</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>284</v>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Alpine A110</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>285</v>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>'06 Honda Civic Si</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>The Hot Ones</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>286</v>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Toyota AE86 Sprinter Trueno</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Ultra Hots</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>287</v>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>Corvette Stingray ('76)</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>Mainlines</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>288</v>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>'18 Ford Mustang RTR Spec 5</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>Silver Series Mustang 60 Years</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>